<commit_message>
finishing touches and presentation
</commit_message>
<xml_diff>
--- a/TonganZhao/PaulShinn/Janus/Flask/static/map-worklist.xlsx
+++ b/TonganZhao/PaulShinn/Janus/Flask/static/map-worklist.xlsx
@@ -894,12 +894,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>33</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -921,12 +921,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>211</t>
+          <t>35</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -948,12 +948,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>213</t>
+          <t>37</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -975,12 +975,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>39</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1002,12 +1002,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>217</t>
+          <t>41</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1029,12 +1029,12 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>43</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1056,12 +1056,12 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>221</t>
+          <t>45</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1083,12 +1083,12 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>223</t>
+          <t>47</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1110,12 +1110,12 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>210</t>
+          <t>34</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1137,12 +1137,12 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>212</t>
+          <t>36</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1164,12 +1164,12 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>214</t>
+          <t>38</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1191,12 +1191,12 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>216</t>
+          <t>40</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1218,12 +1218,12 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>218</t>
+          <t>42</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1245,12 +1245,12 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>44</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1272,12 +1272,12 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>222</t>
+          <t>46</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1299,12 +1299,12 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>224</t>
+          <t>48</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1326,7 +1326,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1353,7 +1353,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1380,7 +1380,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1407,7 +1407,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1434,7 +1434,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1515,7 +1515,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1542,7 +1542,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1569,7 +1569,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1596,7 +1596,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1623,7 +1623,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1650,7 +1650,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1677,7 +1677,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1704,7 +1704,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1731,7 +1731,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1758,12 +1758,12 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>33</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -1785,12 +1785,12 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>211</t>
+          <t>35</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -1812,12 +1812,12 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>213</t>
+          <t>37</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -1839,12 +1839,12 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>39</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -1866,12 +1866,12 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>217</t>
+          <t>41</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -1893,12 +1893,12 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>43</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -1920,12 +1920,12 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>221</t>
+          <t>45</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -1947,12 +1947,12 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>223</t>
+          <t>47</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -1974,12 +1974,12 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>210</t>
+          <t>34</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -2001,12 +2001,12 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>212</t>
+          <t>36</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2028,12 +2028,12 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>214</t>
+          <t>38</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -2055,12 +2055,12 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>216</t>
+          <t>40</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -2082,12 +2082,12 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>218</t>
+          <t>42</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -2109,12 +2109,12 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>44</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2136,12 +2136,12 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>222</t>
+          <t>46</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2163,12 +2163,12 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>224</t>
+          <t>48</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2190,7 +2190,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2217,7 +2217,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2244,7 +2244,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2271,7 +2271,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2298,7 +2298,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2325,7 +2325,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2352,7 +2352,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2379,7 +2379,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2406,7 +2406,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2433,7 +2433,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2460,7 +2460,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2487,7 +2487,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2514,7 +2514,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2568,7 +2568,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2595,7 +2595,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2622,12 +2622,12 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>33</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -2649,12 +2649,12 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>211</t>
+          <t>35</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -2676,12 +2676,12 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>213</t>
+          <t>37</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -2703,12 +2703,12 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>39</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -2730,12 +2730,12 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>217</t>
+          <t>41</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -2757,12 +2757,12 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>43</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -2784,12 +2784,12 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>221</t>
+          <t>45</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -2811,12 +2811,12 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>223</t>
+          <t>47</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -2838,12 +2838,12 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>210</t>
+          <t>34</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -2865,12 +2865,12 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>212</t>
+          <t>36</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -2892,12 +2892,12 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>214</t>
+          <t>38</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -2919,12 +2919,12 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>216</t>
+          <t>40</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -2946,12 +2946,12 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>218</t>
+          <t>42</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -2973,12 +2973,12 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>44</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -3000,12 +3000,12 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>222</t>
+          <t>46</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -3027,12 +3027,12 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>224</t>
+          <t>48</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -3054,7 +3054,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3081,7 +3081,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3108,7 +3108,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3135,7 +3135,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3162,7 +3162,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3189,7 +3189,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3216,7 +3216,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3243,7 +3243,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3270,7 +3270,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3297,7 +3297,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3324,7 +3324,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3351,7 +3351,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3378,7 +3378,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3405,7 +3405,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3432,7 +3432,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3459,7 +3459,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3486,12 +3486,12 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-8</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>33</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
@@ -3513,12 +3513,12 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-8</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>210</t>
+          <t>34</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
@@ -3540,12 +3540,12 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-8</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>211</t>
+          <t>35</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -4103,17 +4103,17 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>A14</t>
+          <t>A03</t>
         </is>
       </c>
     </row>
@@ -4135,17 +4135,17 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>211</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>C14</t>
+          <t>C03</t>
         </is>
       </c>
     </row>
@@ -4167,17 +4167,17 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>213</t>
+          <t>37</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>E14</t>
+          <t>E03</t>
         </is>
       </c>
     </row>
@@ -4199,17 +4199,17 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>G14</t>
+          <t>G03</t>
         </is>
       </c>
     </row>
@@ -4231,17 +4231,17 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>217</t>
+          <t>41</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>I14</t>
+          <t>I03</t>
         </is>
       </c>
     </row>
@@ -4263,17 +4263,17 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>K14</t>
+          <t>K03</t>
         </is>
       </c>
     </row>
@@ -4295,17 +4295,17 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>221</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>M14</t>
+          <t>M03</t>
         </is>
       </c>
     </row>
@@ -4327,17 +4327,17 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>223</t>
+          <t>47</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>O14</t>
+          <t>O03</t>
         </is>
       </c>
     </row>
@@ -4359,17 +4359,17 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>210</t>
+          <t>34</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>B14</t>
+          <t>B03</t>
         </is>
       </c>
     </row>
@@ -4391,17 +4391,17 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>212</t>
+          <t>36</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>D14</t>
+          <t>D03</t>
         </is>
       </c>
     </row>
@@ -4423,17 +4423,17 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>214</t>
+          <t>38</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>F14</t>
+          <t>F03</t>
         </is>
       </c>
     </row>
@@ -4455,17 +4455,17 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>216</t>
+          <t>40</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>H14</t>
+          <t>H03</t>
         </is>
       </c>
     </row>
@@ -4487,17 +4487,17 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>218</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>J14</t>
+          <t>J03</t>
         </is>
       </c>
     </row>
@@ -4519,17 +4519,17 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>L14</t>
+          <t>L03</t>
         </is>
       </c>
     </row>
@@ -4551,17 +4551,17 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>222</t>
+          <t>46</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>N14</t>
+          <t>N03</t>
         </is>
       </c>
     </row>
@@ -4583,17 +4583,17 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>384-1</t>
+          <t>384-2</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>224</t>
+          <t>48</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>P14</t>
+          <t>P03</t>
         </is>
       </c>
     </row>
@@ -4615,7 +4615,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -4647,7 +4647,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -4679,7 +4679,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -4711,7 +4711,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -4743,7 +4743,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -4775,7 +4775,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -4807,7 +4807,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -4839,7 +4839,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -4871,7 +4871,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -4903,7 +4903,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -4935,7 +4935,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -4967,7 +4967,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -4999,7 +4999,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -5031,7 +5031,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -5063,7 +5063,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -5095,7 +5095,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-3</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -5127,17 +5127,17 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>A14</t>
+          <t>A03</t>
         </is>
       </c>
     </row>
@@ -5159,17 +5159,17 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>211</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>C14</t>
+          <t>C03</t>
         </is>
       </c>
     </row>
@@ -5191,17 +5191,17 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>213</t>
+          <t>37</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>E14</t>
+          <t>E03</t>
         </is>
       </c>
     </row>
@@ -5223,17 +5223,17 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>G14</t>
+          <t>G03</t>
         </is>
       </c>
     </row>
@@ -5255,17 +5255,17 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>217</t>
+          <t>41</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>I14</t>
+          <t>I03</t>
         </is>
       </c>
     </row>
@@ -5287,17 +5287,17 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>K14</t>
+          <t>K03</t>
         </is>
       </c>
     </row>
@@ -5319,17 +5319,17 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>221</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>M14</t>
+          <t>M03</t>
         </is>
       </c>
     </row>
@@ -5351,17 +5351,17 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>223</t>
+          <t>47</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>O14</t>
+          <t>O03</t>
         </is>
       </c>
     </row>
@@ -5383,17 +5383,17 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>210</t>
+          <t>34</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>B14</t>
+          <t>B03</t>
         </is>
       </c>
     </row>
@@ -5415,17 +5415,17 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>212</t>
+          <t>36</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>D14</t>
+          <t>D03</t>
         </is>
       </c>
     </row>
@@ -5447,17 +5447,17 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>214</t>
+          <t>38</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>F14</t>
+          <t>F03</t>
         </is>
       </c>
     </row>
@@ -5479,17 +5479,17 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>216</t>
+          <t>40</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>H14</t>
+          <t>H03</t>
         </is>
       </c>
     </row>
@@ -5511,17 +5511,17 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>218</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>J14</t>
+          <t>J03</t>
         </is>
       </c>
     </row>
@@ -5543,17 +5543,17 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>L14</t>
+          <t>L03</t>
         </is>
       </c>
     </row>
@@ -5575,17 +5575,17 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>222</t>
+          <t>46</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>N14</t>
+          <t>N03</t>
         </is>
       </c>
     </row>
@@ -5607,17 +5607,17 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>384-2</t>
+          <t>384-4</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>224</t>
+          <t>48</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>P14</t>
+          <t>P03</t>
         </is>
       </c>
     </row>
@@ -5639,7 +5639,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -5671,7 +5671,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -5703,7 +5703,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -5735,7 +5735,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -5767,7 +5767,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -5799,7 +5799,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -5831,7 +5831,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -5863,7 +5863,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -5895,7 +5895,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -5927,7 +5927,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -5959,7 +5959,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -5991,7 +5991,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -6023,7 +6023,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -6055,7 +6055,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -6087,7 +6087,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -6119,7 +6119,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-5</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -6151,17 +6151,17 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>A14</t>
+          <t>A03</t>
         </is>
       </c>
     </row>
@@ -6183,17 +6183,17 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>211</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>C14</t>
+          <t>C03</t>
         </is>
       </c>
     </row>
@@ -6215,17 +6215,17 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>213</t>
+          <t>37</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>E14</t>
+          <t>E03</t>
         </is>
       </c>
     </row>
@@ -6247,17 +6247,17 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>G14</t>
+          <t>G03</t>
         </is>
       </c>
     </row>
@@ -6279,17 +6279,17 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>217</t>
+          <t>41</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>I14</t>
+          <t>I03</t>
         </is>
       </c>
     </row>
@@ -6311,17 +6311,17 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>K14</t>
+          <t>K03</t>
         </is>
       </c>
     </row>
@@ -6343,17 +6343,17 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>221</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>M14</t>
+          <t>M03</t>
         </is>
       </c>
     </row>
@@ -6375,17 +6375,17 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>223</t>
+          <t>47</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>O14</t>
+          <t>O03</t>
         </is>
       </c>
     </row>
@@ -6407,17 +6407,17 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>210</t>
+          <t>34</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>B14</t>
+          <t>B03</t>
         </is>
       </c>
     </row>
@@ -6439,17 +6439,17 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>212</t>
+          <t>36</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>D14</t>
+          <t>D03</t>
         </is>
       </c>
     </row>
@@ -6471,17 +6471,17 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>214</t>
+          <t>38</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>F14</t>
+          <t>F03</t>
         </is>
       </c>
     </row>
@@ -6503,17 +6503,17 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>216</t>
+          <t>40</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>H14</t>
+          <t>H03</t>
         </is>
       </c>
     </row>
@@ -6535,17 +6535,17 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>218</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>J14</t>
+          <t>J03</t>
         </is>
       </c>
     </row>
@@ -6567,17 +6567,17 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>L14</t>
+          <t>L03</t>
         </is>
       </c>
     </row>
@@ -6599,17 +6599,17 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>222</t>
+          <t>46</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>N14</t>
+          <t>N03</t>
         </is>
       </c>
     </row>
@@ -6631,17 +6631,17 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>384-3</t>
+          <t>384-6</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>224</t>
+          <t>48</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>P14</t>
+          <t>P03</t>
         </is>
       </c>
     </row>
@@ -6663,7 +6663,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -6695,7 +6695,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -6727,7 +6727,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -6759,7 +6759,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -6791,7 +6791,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -6823,7 +6823,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -6855,7 +6855,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -6887,7 +6887,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -6919,7 +6919,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -6951,7 +6951,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
@@ -6983,7 +6983,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
@@ -7015,7 +7015,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -7047,7 +7047,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
@@ -7079,7 +7079,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
@@ -7111,7 +7111,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -7143,7 +7143,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-7</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
@@ -7175,17 +7175,17 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-8</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>A14</t>
+          <t>A03</t>
         </is>
       </c>
     </row>
@@ -7207,17 +7207,17 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-8</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>210</t>
+          <t>34</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>B14</t>
+          <t>B03</t>
         </is>
       </c>
     </row>
@@ -7239,17 +7239,17 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>384-4</t>
+          <t>384-8</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>211</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>C14</t>
+          <t>C03</t>
         </is>
       </c>
     </row>

</xml_diff>